<commit_message>
Se adelantó la estimación de los tiempos de nuevos requerimientos y se agregó el archivo como recurso
</commit_message>
<xml_diff>
--- a/BD/resources/Reporte requerimientos/RequerimientosConfianza.xlsx
+++ b/BD/resources/Reporte requerimientos/RequerimientosConfianza.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samtel\Desktop\Reporte requerimientos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Confianza\BD\resources\Reporte requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A3A0E0-22CE-4EBC-BE42-4EDA0E5717E7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484A31A4-F0A8-4CE7-A613-F25F2BBA70C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2595" yWindow="2595" windowWidth="15375" windowHeight="8325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="05_03_2019" sheetId="1" r:id="rId1"/>
     <sheet name="11_03_2019" sheetId="2" r:id="rId2"/>
     <sheet name="13_03_2019" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="54">
   <si>
     <t>1. Cambio de abreviados</t>
   </si>
@@ -158,9 +158,6 @@
     <t>CORREO AUTOMATICO</t>
   </si>
   <si>
-    <t>50m</t>
-  </si>
-  <si>
     <t>Atar la lista de sector según el número que inicie el codigo CIIU del cliente.</t>
   </si>
   <si>
@@ -171,13 +168,37 @@
   </si>
   <si>
     <t>ALBERT</t>
+  </si>
+  <si>
+    <t>CAPTURA/VERIFICACION</t>
+  </si>
+  <si>
+    <t>TIEMPO TOTAL</t>
+  </si>
+  <si>
+    <t>TIEMPO NATURAL</t>
+  </si>
+  <si>
+    <t>TIEMPO JURIDICO</t>
+  </si>
+  <si>
+    <t>TOTAL HORAS</t>
+  </si>
+  <si>
+    <t>3 DIAS 40 MINUTOS</t>
+  </si>
+  <si>
+    <t>TOTAL DIAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="h:mm:ss;@"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,8 +235,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +260,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,13 +333,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="18">
     <dxf>
       <font>
         <b val="0"/>
@@ -421,6 +484,44 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -512,6 +613,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -552,13 +660,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -693,32 +794,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86FB3DC7-D9FE-4F90-8259-F4DB03B65A2B}" name="Tabla136" displayName="Tabla136" ref="A1:D4" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86FB3DC7-D9FE-4F90-8259-F4DB03B65A2B}" name="Tabla136" displayName="Tabla136" ref="A1:D4" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="A1:D4" xr:uid="{F9EC68DE-BBB1-4F7B-9A48-9FEC68743412}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{56C4D90B-9722-42C1-A165-F0319B043118}" name="REQUERIMIENTOS" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{DBE0A227-0C74-49F5-85B0-7EA8EC9CFD27}" name="COMPLETO" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{10D57CAC-374F-4C10-9E56-4F63C3136E82}" name="TIEMPO" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{B94E23E6-D7ED-4777-9376-813E2882CB7F}" name="NUEVO" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{56C4D90B-9722-42C1-A165-F0319B043118}" name="REQUERIMIENTOS" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{DBE0A227-0C74-49F5-85B0-7EA8EC9CFD27}" name="COMPLETO" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{10D57CAC-374F-4C10-9E56-4F63C3136E82}" name="TIEMPO" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{B94E23E6-D7ED-4777-9376-813E2882CB7F}" name="NUEVO" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D004A61E-D172-49F8-9CB8-5E1D5DEBEE79}" name="Tabla2" displayName="Tabla2" ref="A1:F9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:F9" xr:uid="{DB956E43-47F4-4745-8D3C-CFA9D967AD25}">
-    <filterColumn colId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D004A61E-D172-49F8-9CB8-5E1D5DEBEE79}" name="Tabla2" displayName="Tabla2" ref="A1:H11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:H11" xr:uid="{DB956E43-47F4-4745-8D3C-CFA9D967AD25}">
+    <filterColumn colId="7">
       <filters>
         <filter val="FAIBER"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7ADF8A1D-5F16-4198-AEA9-C2E49811D069}" name="REQUERIMIENTOS" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{E41E42A7-68A7-4DFE-98CB-D25691579ECB}" name="MODULO" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{D9B9DC47-A36E-4E30-A5C3-E211AF888ECA}" name="COMPLETO" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{EE06EEE3-0C2A-4B93-B3DA-3024B867BC16}" name="TIEMPO" dataDxfId="2"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{7ADF8A1D-5F16-4198-AEA9-C2E49811D069}" name="REQUERIMIENTOS" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{E41E42A7-68A7-4DFE-98CB-D25691579ECB}" name="MODULO" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{D9B9DC47-A36E-4E30-A5C3-E211AF888ECA}" name="COMPLETO" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{F8FEAE6B-E9C8-44A2-A004-8C162C455AD6}" name="TIEMPO NATURAL" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{8C69D1D9-994B-4AFD-8110-1831958E9853}" name="TIEMPO JURIDICO" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{EE06EEE3-0C2A-4B93-B3DA-3024B867BC16}" name="TIEMPO TOTAL" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{7E2BBDF6-0C61-4A75-B682-B1A8578DECF9}" name="NUEVO" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{03D098CD-0D34-4DC6-81CA-F069ECB21B38}" name="ASIGNADO A" dataDxfId="0"/>
   </tableColumns>
@@ -1150,22 +1253,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B3448F-F329-47EF-99A5-999BA6262754}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="85.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="75.7109375" style="8" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="15" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="15" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
@@ -1175,17 +1281,23 @@
       <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H1" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
@@ -1195,19 +1307,21 @@
       <c r="C2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="13">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>32</v>
@@ -1215,33 +1329,44 @@
       <c r="C3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="13">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F4" s="13">
+        <f>SUM(Tabla2[[#This Row],[TIEMPO NATURAL]:[TIEMPO JURIDICO]])</f>
+        <v>0.625</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
@@ -1251,15 +1376,24 @@
       <c r="C5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="13">
+        <v>0.125</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F5" s="13">
+        <f>SUM(Tabla2[[#This Row],[TIEMPO NATURAL]:[TIEMPO JURIDICO]])</f>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>35</v>
       </c>
@@ -1270,14 +1404,16 @@
         <v>28</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
@@ -1288,14 +1424,16 @@
         <v>28</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>39</v>
       </c>
@@ -1306,14 +1444,16 @@
         <v>28</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>41</v>
       </c>
@@ -1324,25 +1464,52 @@
         <v>28</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E10" s="19">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F10" s="20">
+        <v>1.1527777777777779</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se cambió la estructura del campo número de planilla en el módulo de radicación
</commit_message>
<xml_diff>
--- a/BD/resources/Reporte requerimientos/RequerimientosConfianza.xlsx
+++ b/BD/resources/Reporte requerimientos/RequerimientosConfianza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Confianza\BD\resources\Reporte requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484A31A4-F0A8-4CE7-A613-F25F2BBA70C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638824C8-C0FA-44A0-9A65-FF4C671C7707}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>1. Cambio de abreviados</t>
   </si>
@@ -196,7 +196,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -335,16 +335,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -354,13 +354,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -613,13 +613,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -658,6 +651,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -807,7 +807,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D004A61E-D172-49F8-9CB8-5E1D5DEBEE79}" name="Tabla2" displayName="Tabla2" ref="A1:H11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D004A61E-D172-49F8-9CB8-5E1D5DEBEE79}" name="Tabla2" displayName="Tabla2" ref="A1:H11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A1:H11" xr:uid="{DB956E43-47F4-4745-8D3C-CFA9D967AD25}">
     <filterColumn colId="7">
       <filters>
@@ -1256,7 +1256,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,7 +1310,7 @@
       <c r="D2" s="13"/>
       <c r="E2" s="14"/>
       <c r="F2" s="13">
-        <v>4.8611111111111112E-2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>15</v>
@@ -1486,7 +1486,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F10" s="20">
-        <v>1.1527777777777779</v>
+        <v>1.2708333333333333</v>
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>

</xml_diff>

<commit_message>
Se agregaron los campos de si o no en el formulario juridico en los campos de verificacion
</commit_message>
<xml_diff>
--- a/BD/resources/Reporte requerimientos/RequerimientosConfianza.xlsx
+++ b/BD/resources/Reporte requerimientos/RequerimientosConfianza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Confianza\BD\resources\Reporte requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638824C8-C0FA-44A0-9A65-FF4C671C7707}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B990E71-4A15-4972-B951-5FDDFA3598C8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>1. Cambio de abreviados</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>TOTAL DIAS</t>
+  </si>
+  <si>
+    <t>OBSERVACIONES</t>
+  </si>
+  <si>
+    <t>El apartado de INFORMACIÓN FINANCIERA no se muestra cuando el estado del formulario es VERIFICACION, teniendo en cuenta que este contiene campos que necesitan verificarse.</t>
   </si>
 </sst>
 </file>
@@ -270,7 +276,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -296,11 +302,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -362,12 +390,103 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -613,6 +732,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -653,13 +779,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -794,20 +913,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86FB3DC7-D9FE-4F90-8259-F4DB03B65A2B}" name="Tabla136" displayName="Tabla136" ref="A1:D4" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86FB3DC7-D9FE-4F90-8259-F4DB03B65A2B}" name="Tabla136" displayName="Tabla136" ref="A1:D4" totalsRowShown="0" headerRowDxfId="22">
   <autoFilter ref="A1:D4" xr:uid="{F9EC68DE-BBB1-4F7B-9A48-9FEC68743412}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{56C4D90B-9722-42C1-A165-F0319B043118}" name="REQUERIMIENTOS" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{DBE0A227-0C74-49F5-85B0-7EA8EC9CFD27}" name="COMPLETO" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{10D57CAC-374F-4C10-9E56-4F63C3136E82}" name="TIEMPO" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{B94E23E6-D7ED-4777-9376-813E2882CB7F}" name="NUEVO" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{56C4D90B-9722-42C1-A165-F0319B043118}" name="REQUERIMIENTOS" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{DBE0A227-0C74-49F5-85B0-7EA8EC9CFD27}" name="COMPLETO" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{10D57CAC-374F-4C10-9E56-4F63C3136E82}" name="TIEMPO" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{B94E23E6-D7ED-4777-9376-813E2882CB7F}" name="NUEVO" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D004A61E-D172-49F8-9CB8-5E1D5DEBEE79}" name="Tabla2" displayName="Tabla2" ref="A1:H11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D004A61E-D172-49F8-9CB8-5E1D5DEBEE79}" name="Tabla2" displayName="Tabla2" ref="A1:H11" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:H11" xr:uid="{DB956E43-47F4-4745-8D3C-CFA9D967AD25}">
     <filterColumn colId="7">
       <filters>
@@ -816,14 +935,25 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{7ADF8A1D-5F16-4198-AEA9-C2E49811D069}" name="REQUERIMIENTOS" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{E41E42A7-68A7-4DFE-98CB-D25691579ECB}" name="MODULO" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{D9B9DC47-A36E-4E30-A5C3-E211AF888ECA}" name="COMPLETO" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{F8FEAE6B-E9C8-44A2-A004-8C162C455AD6}" name="TIEMPO NATURAL" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{8C69D1D9-994B-4AFD-8110-1831958E9853}" name="TIEMPO JURIDICO" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{EE06EEE3-0C2A-4B93-B3DA-3024B867BC16}" name="TIEMPO TOTAL" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{7E2BBDF6-0C61-4A75-B682-B1A8578DECF9}" name="NUEVO" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{03D098CD-0D34-4DC6-81CA-F069ECB21B38}" name="ASIGNADO A" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{7ADF8A1D-5F16-4198-AEA9-C2E49811D069}" name="REQUERIMIENTOS" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{E41E42A7-68A7-4DFE-98CB-D25691579ECB}" name="MODULO" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{D9B9DC47-A36E-4E30-A5C3-E211AF888ECA}" name="COMPLETO" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{F8FEAE6B-E9C8-44A2-A004-8C162C455AD6}" name="TIEMPO NATURAL" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{8C69D1D9-994B-4AFD-8110-1831958E9853}" name="TIEMPO JURIDICO" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{EE06EEE3-0C2A-4B93-B3DA-3024B867BC16}" name="TIEMPO TOTAL" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{7E2BBDF6-0C61-4A75-B682-B1A8578DECF9}" name="NUEVO" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{03D098CD-0D34-4DC6-81CA-F069ECB21B38}" name="ASIGNADO A" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{275C204B-7C9F-4B8B-B277-4BEA047759EC}" name="Tabla3" displayName="Tabla3" ref="A15:B16" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="3" tableBorderDxfId="4">
+  <autoFilter ref="A15:B16" xr:uid="{CC38916F-B774-46BB-93CD-6F6617E3E907}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{784DD1E2-D105-49CE-8DA8-526C324C531A}" name="REQUERIMIENTOS" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{DE818255-D0DF-4A08-9DD1-6C7A51B910E6}" name="OBSERVACIONES" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1253,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B3448F-F329-47EF-99A5-999BA6262754}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,7 +1435,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="14"/>
@@ -1505,11 +1635,28 @@
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
     </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>